<commit_message>
Add support of Tyva BMS
</commit_message>
<xml_diff>
--- a/deploy/Server.xlsx
+++ b/deploy/Server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\leshan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benoit\Documents\Development\Sheeld\leshan\deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{813B3684-8123-45CC-B786-5BF0023F7EAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964CDC07-900C-470F-8E20-E1E0F4889875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{76A129FA-FE88-4F46-A926-0E901B8C8AFD}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{76A129FA-FE88-4F46-A926-0E901B8C8AFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>HTTP port</t>
   </si>
@@ -48,10 +48,22 @@
     <t>Coap secure Port</t>
   </si>
   <si>
-    <t>http://demo.iot.sheeld.co</t>
-  </si>
-  <si>
-    <t>http://mehariclub.iot.sheeld.co</t>
+    <t>https://demo.iot.sheeld.co</t>
+  </si>
+  <si>
+    <t>https://mehariclub.iot.sheeld.co</t>
+  </si>
+  <si>
+    <t>https://admin.iot.sheeld.co</t>
+  </si>
+  <si>
+    <t>https://v-mti.iot.sheeld.co</t>
+  </si>
+  <si>
+    <t>https://tyva.iot.sheeld.co</t>
+  </si>
+  <si>
+    <t>Short ID</t>
   </si>
 </sst>
 </file>
@@ -414,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1C21CE-4E97-419E-AD3D-4B682ED2D508}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,7 +438,7 @@
     <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -439,39 +451,99 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>8079</v>
+      </c>
+      <c r="C2">
+        <v>5681</v>
+      </c>
+      <c r="D2">
+        <v>5682</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>8080</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>5683</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>5684</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>8081</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>5685</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>5686</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>8082</v>
+      </c>
+      <c r="C5">
+        <v>5687</v>
+      </c>
+      <c r="D5">
+        <v>5688</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>8083</v>
+      </c>
+      <c r="C6">
+        <v>5689</v>
+      </c>
+      <c r="D6">
+        <v>5690</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{DB0C8F98-8175-4069-87A8-7563140357CF}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{59642139-26C1-43D7-9843-D3B69D5219CA}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{DB0C8F98-8175-4069-87A8-7563140357CF}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{59642139-26C1-43D7-9843-D3B69D5219CA}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{10ECC4B7-6F7F-4848-8161-2DFDFC81E608}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{D1B640E4-FCEB-498D-88A8-893480C52EAD}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{2D12E864-9A84-499F-93BD-9A130C8ACBB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>